<commit_message>
Inmplemented a solution on reading the input not the formula from Exel and changing BaseEntity to Identity from Sequance
</commit_message>
<xml_diff>
--- a/data/TestData.xlsx
+++ b/data/TestData.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="32">
   <si>
     <t>henry</t>
   </si>
@@ -106,6 +106,15 @@
   </si>
   <si>
     <t>Seller</t>
+  </si>
+  <si>
+    <t>Test11</t>
+  </si>
+  <si>
+    <t>Test111</t>
+  </si>
+  <si>
+    <t>TestCompany</t>
   </si>
 </sst>
 </file>
@@ -423,10 +432,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F9"/>
+  <dimension ref="A1:F12"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -611,6 +620,77 @@
         <v>2500</v>
       </c>
     </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>29</v>
+      </c>
+      <c r="B10" t="s">
+        <v>30</v>
+      </c>
+      <c r="C10">
+        <v>1111</v>
+      </c>
+      <c r="D10" t="s">
+        <v>31</v>
+      </c>
+      <c r="E10" t="s">
+        <v>25</v>
+      </c>
+      <c r="F10">
+        <v>250005</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A11" t="str">
+        <f>A10</f>
+        <v>Test11</v>
+      </c>
+      <c r="B11" t="str">
+        <f>B10</f>
+        <v>Test111</v>
+      </c>
+      <c r="C11">
+        <f>C8</f>
+        <v>23</v>
+      </c>
+      <c r="D11" t="str">
+        <f>D3</f>
+        <v>Facebook</v>
+      </c>
+      <c r="E11" t="str">
+        <f>E4</f>
+        <v>Hardware E</v>
+      </c>
+      <c r="F11">
+        <f>F5</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A12" t="str">
+        <f>A2</f>
+        <v>henry</v>
+      </c>
+      <c r="B12" t="str">
+        <f>B4</f>
+        <v>Netzov</v>
+      </c>
+      <c r="C12">
+        <v>23</v>
+      </c>
+      <c r="D12" t="str">
+        <f>D3</f>
+        <v>Facebook</v>
+      </c>
+      <c r="E12" t="str">
+        <f>E11</f>
+        <v>Hardware E</v>
+      </c>
+      <c r="F12">
+        <f>F6</f>
+        <v>1111</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Working functionality CreateXML File and ADD his Value from Database
</commit_message>
<xml_diff>
--- a/data/TestData.xlsx
+++ b/data/TestData.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="33">
   <si>
     <t>henry</t>
   </si>
@@ -96,9 +96,6 @@
     <t>Alpha</t>
   </si>
   <si>
-    <t>Test</t>
-  </si>
-  <si>
     <t>Testov</t>
   </si>
   <si>
@@ -108,13 +105,19 @@
     <t>Seller</t>
   </si>
   <si>
-    <t>Test11</t>
-  </si>
-  <si>
-    <t>Test111</t>
-  </si>
-  <si>
-    <t>TestCompany</t>
+    <t>Vesselin</t>
+  </si>
+  <si>
+    <t>Nokia</t>
+  </si>
+  <si>
+    <t>Developer</t>
+  </si>
+  <si>
+    <t>DDD</t>
+  </si>
+  <si>
+    <t>Test1</t>
   </si>
 </sst>
 </file>
@@ -432,10 +435,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F12"/>
+  <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -562,19 +565,19 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
+        <v>32</v>
+      </c>
+      <c r="B7" t="s">
         <v>25</v>
-      </c>
-      <c r="B7" t="s">
-        <v>26</v>
       </c>
       <c r="C7">
         <v>23</v>
       </c>
       <c r="D7" t="s">
+        <v>26</v>
+      </c>
+      <c r="E7" t="s">
         <v>27</v>
-      </c>
-      <c r="E7" t="s">
-        <v>28</v>
       </c>
       <c r="F7">
         <v>1111</v>
@@ -582,19 +585,19 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
+        <v>32</v>
+      </c>
+      <c r="B8" t="s">
         <v>25</v>
-      </c>
-      <c r="B8" t="s">
-        <v>26</v>
       </c>
       <c r="C8">
         <v>23</v>
       </c>
       <c r="D8" t="s">
+        <v>26</v>
+      </c>
+      <c r="E8" t="s">
         <v>27</v>
-      </c>
-      <c r="E8" t="s">
-        <v>28</v>
       </c>
       <c r="F8">
         <v>1111</v>
@@ -622,73 +625,43 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
+        <v>28</v>
+      </c>
+      <c r="B10" t="s">
+        <v>5</v>
+      </c>
+      <c r="C10">
+        <v>51</v>
+      </c>
+      <c r="D10" t="s">
         <v>29</v>
       </c>
-      <c r="B10" t="s">
+      <c r="E10" t="s">
         <v>30</v>
       </c>
-      <c r="C10">
-        <v>1111</v>
-      </c>
-      <c r="D10" t="s">
-        <v>31</v>
-      </c>
-      <c r="E10" t="s">
-        <v>25</v>
-      </c>
       <c r="F10">
-        <v>250005</v>
+        <v>5000</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" t="str">
-        <f>A10</f>
-        <v>Test11</v>
-      </c>
-      <c r="B11" t="str">
-        <f>B10</f>
-        <v>Test111</v>
+        <f>A7</f>
+        <v>Test1</v>
+      </c>
+      <c r="B11" t="s">
+        <v>5</v>
       </c>
       <c r="C11">
-        <f>C8</f>
+        <v>111</v>
+      </c>
+      <c r="D11" t="s">
         <v>23</v>
       </c>
-      <c r="D11" t="str">
-        <f>D3</f>
-        <v>Facebook</v>
-      </c>
-      <c r="E11" t="str">
-        <f>E4</f>
-        <v>Hardware E</v>
+      <c r="E11" t="s">
+        <v>31</v>
       </c>
       <c r="F11">
-        <f>F5</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A12" t="str">
-        <f>A2</f>
-        <v>henry</v>
-      </c>
-      <c r="B12" t="str">
-        <f>B4</f>
-        <v>Netzov</v>
-      </c>
-      <c r="C12">
-        <v>23</v>
-      </c>
-      <c r="D12" t="str">
-        <f>D3</f>
-        <v>Facebook</v>
-      </c>
-      <c r="E12" t="str">
-        <f>E11</f>
-        <v>Hardware E</v>
-      </c>
-      <c r="F12">
-        <f>F6</f>
-        <v>1111</v>
+        <v>111</v>
       </c>
     </row>
   </sheetData>

</xml_diff>